<commit_message>
Add Emuart class, fix communication stability
</commit_message>
<xml_diff>
--- a/emulator_adresses_and_command.xlsx
+++ b/emulator_adresses_and_command.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pokpong.c\Desktop\emu-LLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A851CA-E869-490F-87A7-D3452ABA0354}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0E759A-C265-4F5C-8334-77FE1FA14BC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2580" yWindow="5565" windowWidth="30030" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Address</t>
   </si>
@@ -33,9 +33,6 @@
     <t>0x7E</t>
   </si>
   <si>
-    <t>Start Byte</t>
-  </si>
-  <si>
     <t>0x00 - 0xFF</t>
   </si>
   <si>
@@ -64,6 +61,81 @@
   </si>
   <si>
     <t>Dataframe (1Mbps 8N1)</t>
+  </si>
+  <si>
+    <t>0x77</t>
+  </si>
+  <si>
+    <t>Start Bytes</t>
+  </si>
+  <si>
+    <t>Control LD3</t>
+  </si>
+  <si>
+    <t>0x93</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Control LD4</t>
+  </si>
+  <si>
+    <t>0x94</t>
+  </si>
+  <si>
+    <t>0xAF</t>
+  </si>
+  <si>
+    <t>0xA0</t>
+  </si>
+  <si>
+    <t>0x74</t>
+  </si>
+  <si>
+    <t>0xE3</t>
+  </si>
+  <si>
+    <t>0x45</t>
+  </si>
+  <si>
+    <t>0xA2</t>
+  </si>
+  <si>
+    <t>0xB6</t>
+  </si>
+  <si>
+    <t>0xBB</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>0xDF</t>
+  </si>
+  <si>
+    <t>0xD0</t>
+  </si>
+  <si>
+    <t>0x31</t>
+  </si>
+  <si>
+    <t>0xC4</t>
+  </si>
+  <si>
+    <t>0xE1</t>
+  </si>
+  <si>
+    <t>0x40</t>
   </si>
 </sst>
 </file>
@@ -100,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -123,23 +195,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,87 +511,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K4"/>
+  <dimension ref="A2:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="13.28515625" style="3"/>
+    <col min="1" max="16384" width="13.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="J4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>8</v>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H3:K3"/>
+  <mergeCells count="11">
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add emuPeripheral.h and polish some code
</commit_message>
<xml_diff>
--- a/emulator_adresses_and_command.xlsx
+++ b/emulator_adresses_and_command.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pokpong.c\Desktop\emu-LLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0E759A-C265-4F5C-8334-77FE1FA14BC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24CDF008-DA82-47A9-9101-35503FB6BA32}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="5565" windowWidth="30030" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="5910" windowWidth="30030" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
-  <si>
-    <t>Address</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>0x7E</t>
   </si>
@@ -136,13 +134,25 @@
   </si>
   <si>
     <t>0x40</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>EEPROM</t>
+  </si>
+  <si>
+    <t>0x66</t>
+  </si>
+  <si>
+    <t>Write</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,16 +173,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -196,19 +255,215 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -216,24 +471,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -511,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L14"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -522,62 +826,66 @@
     <col min="1" max="16384" width="13.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="1" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
+    </row>
+    <row r="3" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
@@ -587,175 +895,303 @@
       <c r="K4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="3"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>27</v>
+      <c r="F19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="20">
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:L18"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="F14:H14"/>
+    <mergeCell ref="E4:G4"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New emu-LLC code initial commit
</commit_message>
<xml_diff>
--- a/emulator_adresses_and_command.xlsx
+++ b/emulator_adresses_and_command.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pokpong.c\Desktop\emu-LLC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szgno\Desktop\emu-LLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D53515-DE79-459F-919E-179FF7E27C27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859F3E51-A234-4157-A930-A151D9FAA3F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="8865" windowWidth="30030" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7710" yWindow="3375" windowWidth="20250" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="100">
   <si>
     <t>0x7E</t>
   </si>
@@ -172,6 +180,159 @@
   </si>
   <si>
     <t>0x10</t>
+  </si>
+  <si>
+    <t>Actuator</t>
+  </si>
+  <si>
+    <t>Open Loop Speed</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>Single Precision Float</t>
+  </si>
+  <si>
+    <t>Joint [N]</t>
+  </si>
+  <si>
+    <t>uint8_t</t>
+  </si>
+  <si>
+    <t>microstep</t>
+  </si>
+  <si>
+    <t>0xN1</t>
+  </si>
+  <si>
+    <t>0xN2</t>
+  </si>
+  <si>
+    <t>0xN3</t>
+  </si>
+  <si>
+    <t>0xN4</t>
+  </si>
+  <si>
+    <t>0xN5</t>
+  </si>
+  <si>
+    <t>0xN6</t>
+  </si>
+  <si>
+    <t>0xN7</t>
+  </si>
+  <si>
+    <t>0xN8</t>
+  </si>
+  <si>
+    <t>0xN9</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>max_velocity [rad/s]</t>
+  </si>
+  <si>
+    <t>lower_joint_limit [rad]</t>
+  </si>
+  <si>
+    <t>upper_joint_limit [rad]</t>
+  </si>
+  <si>
+    <t>gear_ratio (speed reduced from motor shaft to encoder)</t>
+  </si>
+  <si>
+    <t>ols*gear_ratio*microstep*200/(2pi)</t>
+  </si>
+  <si>
+    <t>0x4&lt;JointNum&gt;</t>
+  </si>
+  <si>
+    <t>0x5&lt;JointNum&gt;</t>
+  </si>
+  <si>
+    <t>4 Bytes (Velocity in radiant)</t>
+  </si>
+  <si>
+    <t>Jog in Configuration Space</t>
+  </si>
+  <si>
+    <t>0x6&lt;JointNum&gt;</t>
+  </si>
+  <si>
+    <t>0x7&lt;JointNum&gt;</t>
+  </si>
+  <si>
+    <t>Jog in Task Space</t>
+  </si>
+  <si>
+    <t>6 Increment in meter, radiant and 6 duration</t>
+  </si>
+  <si>
+    <t>q1, q2 ,… ,q6 and T1, T2, …, T6</t>
+  </si>
+  <si>
+    <t>Single-Joint Command</t>
+  </si>
+  <si>
+    <t>Follow Trajectory</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0x8&lt;JointNum&gt;</t>
+  </si>
+  <si>
+    <t>q1p1, q2p1 ,… ,q6p1 and q1p2, q2p2 ,… ,q6p2, ... and v1p1, v2p1, …, v6p1 and v1p2, v2p2, …, v6p2 and T1, T2, …, T6</t>
+  </si>
+  <si>
+    <t>&lt;NumPoint&gt; x 12 (position, velocity) + &lt;NumPoint&gt;-1 (duration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;NumPoint&gt; x 12  + &lt;NumPoint&gt;-1 </t>
+  </si>
+  <si>
+    <t>Can't run while controller is initialized</t>
+  </si>
+  <si>
+    <t>8 Bytes (Increment in radiant and duration in second)</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>Absolute Joint Position</t>
+  </si>
+  <si>
+    <t>9 Bytes (Increment in radiant and duration in second)</t>
+  </si>
+  <si>
+    <t>Joint State</t>
+  </si>
+  <si>
+    <t>6 Bytes (Joint Position) + 2 Bytes (Status Bytes)</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>Simple Joint State</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>6 Bytes (Joint Position) + 6 Bytes (Joint Velocity) + 2 Bytes (Status Bytes)</t>
+  </si>
+  <si>
+    <t>Full Joint State</t>
   </si>
 </sst>
 </file>
@@ -229,7 +390,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -504,7 +671,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -539,6 +706,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -548,18 +760,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,17 +775,44 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -865,57 +1098,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="13.28515625" style="1"/>
+    <col min="1" max="1" width="26.28515625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" style="1"/>
+    <col min="4" max="4" width="22.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="1"/>
+    <col min="7" max="7" width="28.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="13.28515625" style="1"/>
+    <col min="13" max="13" width="66" style="1" customWidth="1"/>
+    <col min="14" max="15" width="13.28515625" style="1"/>
+    <col min="16" max="16" width="11.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="54.7109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="13.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+    <row r="1" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="21"/>
-    </row>
-    <row r="3" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
+      <c r="O2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="22" t="s">
+      <c r="F3" s="35"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="23"/>
-    </row>
-    <row r="4" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="26"/>
+      <c r="O3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -928,11 +1179,11 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
@@ -945,12 +1196,27 @@
       <c r="K4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="O5" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
@@ -961,37 +1227,44 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
     </row>
-    <row r="6" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
+    <row r="6" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="15"/>
+      <c r="O6" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
     </row>
-    <row r="7" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="25" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="13" t="s">
         <v>45</v>
       </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
+      <c r="O7" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
@@ -999,32 +1272,39 @@
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
     </row>
-    <row r="8" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
+    <row r="8" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36"/>
+      <c r="B8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="38"/>
+      <c r="D8" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="12" t="s">
+      <c r="G8" s="42"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="14"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
+      <c r="O8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -1035,7 +1315,7 @@
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1051,11 +1331,11 @@
       <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1069,9 +1349,15 @@
         <v>35</v>
       </c>
       <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
+      <c r="O9" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>68</v>
+      </c>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
@@ -1082,7 +1368,7 @@
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
     </row>
-    <row r="10" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1098,11 +1384,11 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1115,42 +1401,58 @@
       <c r="L10" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:26" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="O10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q11" s="17"/>
+    </row>
+    <row r="12" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O12" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="13" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="25" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+    <row r="14" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
+      <c r="B14" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="38"/>
+      <c r="D14" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="12" t="s">
+      <c r="G14" s="42"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="14"/>
-    </row>
-    <row r="15" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="43"/>
+    </row>
+    <row r="15" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
@@ -1166,11 +1468,11 @@
       <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1184,7 +1486,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1200,11 +1502,11 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1218,41 +1520,42 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+    <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="25" t="s">
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
+    <row r="20" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="38"/>
+      <c r="D20" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="12" t="s">
+      <c r="G20" s="42"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="14"/>
-    </row>
-    <row r="21" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="43"/>
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -1268,11 +1571,11 @@
       <c r="E21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
       <c r="I21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1286,42 +1589,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+    <row r="23" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="25" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="22" t="s">
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
+      <c r="B25" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="6" t="s">
+      <c r="C25" s="38"/>
+      <c r="D25" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="12" t="s">
+      <c r="G25" s="42"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="14"/>
-    </row>
-    <row r="26" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="43"/>
+    </row>
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="6" t="s">
         <v>0</v>
@@ -1335,11 +1638,11 @@
       <c r="E26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="6" t="s">
         <v>3</v>
       </c>
@@ -1353,37 +1656,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+    <row r="28" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="25" t="s">
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="22" t="s">
+    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="39"/>
+      <c r="B30" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="9" t="s">
+      <c r="C30" s="38"/>
+      <c r="D30" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="43"/>
+    </row>
+    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9" t="s">
         <v>0</v>
@@ -1410,42 +1713,386 @@
         <v>6</v>
       </c>
     </row>
+    <row r="33" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="38"/>
+      <c r="D35" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="G35" s="42"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="43"/>
+    </row>
+    <row r="36" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="G36" s="28"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N36" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+    </row>
+    <row r="37" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="28"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="28"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="L38" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="G39" s="28"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="46"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="L40" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M40" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+    </row>
+    <row r="44" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="36"/>
+      <c r="B44" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="38"/>
+      <c r="D44" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44" s="42"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="42"/>
+      <c r="K44" s="42"/>
+      <c r="L44" s="43"/>
+    </row>
+    <row r="45" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G45" s="28"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="L45" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F46" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G46" s="46"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="K46" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="L46" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="49">
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F39:H39"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="I14:L14"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="F26:H26"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="I25:L25"/>
-    <mergeCell ref="F26:H26"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:L20"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="R7:T7"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="U6:X6"/>
-    <mergeCell ref="N6:O6"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="I35:L35"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add emulator's target file
</commit_message>
<xml_diff>
--- a/emulator_adresses_and_command.xlsx
+++ b/emulator_adresses_and_command.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szgno\Desktop\emu-LLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3982BEE9-76F4-4A19-8705-AAFA32030007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C816BE23-239A-4BB5-943F-3222A2CA8086}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-7500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="126">
   <si>
     <t>0x7E</t>
   </si>
@@ -818,7 +818,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -916,91 +916,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1287,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z64"/>
+  <dimension ref="A1:AA64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1299,63 +1314,66 @@
     <col min="2" max="3" width="13.28515625" style="1"/>
     <col min="4" max="4" width="22.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="1"/>
-    <col min="7" max="7" width="28.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
-    <col min="9" max="12" width="13.28515625" style="1"/>
-    <col min="13" max="13" width="66" style="1" customWidth="1"/>
-    <col min="14" max="15" width="13.28515625" style="1"/>
-    <col min="16" max="16" width="11.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="54.7109375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="13.28515625" style="1"/>
+    <col min="6" max="6" width="19" style="33" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1"/>
+    <col min="8" max="8" width="28.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
+    <col min="10" max="13" width="13.28515625" style="1"/>
+    <col min="14" max="14" width="66" style="1" customWidth="1"/>
+    <col min="15" max="16" width="13.28515625" style="1"/>
+    <col min="17" max="17" width="11.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="54.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="13.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+    <row r="1" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-      <c r="O2" s="1" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="58"/>
+      <c r="P2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="53" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="54"/>
-      <c r="O3" s="1" t="s">
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="60"/>
+      <c r="P3" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1368,133 +1386,134 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="2" t="s">
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="R4" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N5" s="4"/>
-      <c r="O5" s="16" t="s">
+    <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="4"/>
+      <c r="P5" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="Q5" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="R5" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
-      <c r="Y5" s="5"/>
+      <c r="Y5" s="4"/>
       <c r="Z5" s="5"/>
-    </row>
-    <row r="6" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N6" s="15"/>
-      <c r="O6" s="16" t="s">
+      <c r="AA5" s="5"/>
+    </row>
+    <row r="6" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O6" s="15"/>
+      <c r="P6" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="5"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
       <c r="Z6" s="5"/>
-    </row>
-    <row r="7" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="AA6" s="5"/>
+    </row>
+    <row r="7" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="5"/>
+      <c r="P7" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="Q7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="R7" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="5"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA7" s="5"/>
+    </row>
+    <row r="8" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="41"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="41"/>
+      <c r="G8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="33" t="s">
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="35"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="16" t="s">
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="41"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="R8" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
@@ -1503,8 +1522,9 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-    </row>
-    <row r="9" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA8" s="10"/>
+    </row>
+    <row r="9" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1520,34 +1540,34 @@
       <c r="E9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="36"/>
+      <c r="G9" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="2" t="s">
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="5"/>
+      <c r="P9" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="P9" s="11" t="s">
+      <c r="Q9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="19" t="s">
+      <c r="R9" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
@@ -1556,8 +1576,9 @@
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
-    </row>
-    <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA9" s="5"/>
+    </row>
+    <row r="10" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1573,75 +1594,77 @@
       <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="36"/>
+      <c r="G10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="2" t="s">
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="16" t="s">
+      <c r="P10" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="Q10" s="17"/>
-    </row>
-    <row r="11" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O11" s="16" t="s">
+      <c r="R10" s="17"/>
+    </row>
+    <row r="11" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="Q11" s="17"/>
-    </row>
-    <row r="12" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O12" s="16" t="s">
+      <c r="R11" s="17"/>
+    </row>
+    <row r="12" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="Q12" s="17"/>
-    </row>
-    <row r="13" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="R12" s="17"/>
+    </row>
+    <row r="13" spans="1:27" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
       <c r="D13" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="41"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="41"/>
+      <c r="G14" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="33" t="s">
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
-    </row>
-    <row r="15" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+    </row>
+    <row r="15" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
@@ -1657,25 +1680,26 @@
       <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="46" t="s">
+      <c r="F15" s="36"/>
+      <c r="G15" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="2" t="s">
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1691,60 +1715,63 @@
       <c r="E16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="36"/>
+      <c r="G16" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="2" t="s">
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+    <row r="17" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="33"/>
+    </row>
+    <row r="19" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="41"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="41"/>
+      <c r="G19" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="33" t="s">
+      <c r="H19" s="40"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="35"/>
-    </row>
-    <row r="20" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+    </row>
+    <row r="20" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>17</v>
       </c>
@@ -1760,25 +1787,26 @@
       <c r="E20" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="36"/>
+      <c r="G20" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="30" t="s">
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="30" t="s">
+      <c r="K20" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="K20" s="30" t="s">
+      <c r="L20" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="30" t="s">
+      <c r="M20" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -1794,81 +1822,85 @@
       <c r="E21" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="46" t="s">
+      <c r="F21" s="36"/>
+      <c r="G21" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="30" t="s">
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="J21" s="30" t="s">
+      <c r="K21" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="K21" s="30" t="s">
+      <c r="L21" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="L21" s="30" t="s">
+      <c r="M21" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
       <c r="L22" s="29"/>
-    </row>
-    <row r="23" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="37" t="s">
+      <c r="M22" s="29"/>
+    </row>
+    <row r="23" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="13" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="32"/>
       <c r="H23" s="32"/>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>
-    </row>
-    <row r="24" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="32"/>
+    </row>
+    <row r="24" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="41"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="41"/>
+      <c r="G24" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="33" t="s">
+      <c r="H24" s="40"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="35"/>
-    </row>
-    <row r="25" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="41"/>
+    </row>
+    <row r="25" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>17</v>
       </c>
@@ -1884,25 +1916,26 @@
       <c r="E25" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="36"/>
+      <c r="G25" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="31" t="s">
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="J25" s="31" t="s">
+      <c r="K25" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="31" t="s">
+      <c r="L25" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="L25" s="31" t="s">
+      <c r="M25" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
@@ -1918,77 +1951,80 @@
       <c r="E26" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="46" t="s">
+      <c r="F26" s="36"/>
+      <c r="G26" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="31" t="s">
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="K26" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="K26" s="31" t="s">
+      <c r="L26" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="L26" s="31" t="s">
+      <c r="M26" s="31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" s="28" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="F27" s="35"/>
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29"/>
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
-    </row>
-    <row r="28" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
+      <c r="M27" s="29"/>
+    </row>
+    <row r="28" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="49"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="65"/>
       <c r="D28" s="13" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
-    </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="28"/>
+    </row>
+    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="57"/>
+      <c r="C29" s="55"/>
       <c r="D29" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="41"/>
+      <c r="G29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="33" t="s">
+      <c r="H29" s="40"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="35"/>
-    </row>
-    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="41"/>
+    </row>
+    <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>39</v>
       </c>
@@ -2004,60 +2040,62 @@
       <c r="E30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="42" t="s">
+      <c r="F30" s="34"/>
+      <c r="G30" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="2" t="s">
+      <c r="H30" s="46"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="37" t="s">
+    <row r="32" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="39"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="41"/>
+      <c r="C34" s="44"/>
       <c r="D34" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="33" t="s">
+      <c r="F34" s="41"/>
+      <c r="G34" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="33" t="s">
+      <c r="H34" s="40"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="35"/>
-    </row>
-    <row r="35" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="41"/>
+    </row>
+    <row r="35" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="6" t="s">
         <v>0</v>
@@ -2071,55 +2109,57 @@
       <c r="E35" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F35" s="42" t="s">
+      <c r="F35" s="34"/>
+      <c r="G35" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="43"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="6" t="s">
+      <c r="H35" s="46"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="K35" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="L35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L35" s="6" t="s">
+      <c r="M35" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
+    <row r="37" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="39"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="53"/>
       <c r="D38" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="41"/>
+      <c r="C39" s="44"/>
       <c r="D39" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E39" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="33" t="s">
+      <c r="F39" s="41"/>
+      <c r="G39" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="35"/>
-    </row>
-    <row r="40" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="41"/>
+    </row>
+    <row r="40" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="9" t="s">
         <v>0</v>
@@ -2133,55 +2173,57 @@
       <c r="E40" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="36"/>
+      <c r="G40" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="H40" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="I40" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I40" s="9" t="s">
+      <c r="J40" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="37" t="s">
+    <row r="42" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="39"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="53"/>
       <c r="D43" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="41"/>
+      <c r="C44" s="44"/>
       <c r="D44" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="25" t="s">
+      <c r="E44" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F44" s="33" t="s">
+      <c r="F44" s="41"/>
+      <c r="G44" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="G44" s="34"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="33" t="s">
+      <c r="H44" s="40"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J44" s="34"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="35"/>
-    </row>
-    <row r="45" spans="1:16" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="41"/>
+    </row>
+    <row r="45" spans="1:17" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>83</v>
       </c>
@@ -2197,51 +2239,53 @@
       <c r="E45" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F45" s="42" t="s">
+      <c r="F45" s="34"/>
+      <c r="G45" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="G45" s="43"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="22" t="s">
+      <c r="H45" s="46"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="J45" s="22" t="s">
+      <c r="K45" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K45" s="22" t="s">
+      <c r="L45" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L45" s="22" t="s">
+      <c r="M45" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="40" t="s">
+      <c r="B46" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="41"/>
+      <c r="C46" s="44"/>
       <c r="D46" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E46" s="25" t="s">
+      <c r="E46" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F46" s="33" t="s">
+      <c r="F46" s="41"/>
+      <c r="G46" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="G46" s="34"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="33" t="s">
+      <c r="H46" s="40"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="35"/>
-    </row>
-    <row r="47" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="41"/>
+    </row>
+    <row r="47" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>50</v>
       </c>
@@ -2257,33 +2301,34 @@
       <c r="E47" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F47" s="42" t="s">
+      <c r="F47" s="34"/>
+      <c r="G47" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="G47" s="43"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="14" t="s">
+      <c r="H47" s="46"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J47" s="14" t="s">
+      <c r="K47" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K47" s="14" t="s">
+      <c r="L47" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L47" s="14" t="s">
+      <c r="M47" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N47" s="36" t="s">
+      <c r="O47" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="O47" s="36"/>
-      <c r="P47" s="36"/>
-    </row>
-    <row r="48" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P47" s="66"/>
+      <c r="Q47" s="66"/>
+    </row>
+    <row r="48" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>97</v>
       </c>
@@ -2299,25 +2344,26 @@
       <c r="E48" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="42" t="s">
+      <c r="F48" s="34"/>
+      <c r="G48" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="G48" s="43"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="12" t="s">
+      <c r="H48" s="46"/>
+      <c r="I48" s="47"/>
+      <c r="J48" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J48" s="12" t="s">
+      <c r="K48" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K48" s="12" t="s">
+      <c r="L48" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L48" s="12" t="s">
+      <c r="M48" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>98</v>
       </c>
@@ -2333,25 +2379,26 @@
       <c r="E49" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F49" s="42" t="s">
+      <c r="F49" s="34"/>
+      <c r="G49" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="G49" s="43"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="14" t="s">
+      <c r="H49" s="46"/>
+      <c r="I49" s="47"/>
+      <c r="J49" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J49" s="14" t="s">
+      <c r="K49" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K49" s="14" t="s">
+      <c r="L49" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L49" s="14" t="s">
+      <c r="M49" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>99</v>
       </c>
@@ -2367,28 +2414,29 @@
       <c r="E50" s="14">
         <v>28</v>
       </c>
-      <c r="F50" s="42" t="s">
+      <c r="F50" s="34"/>
+      <c r="G50" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="G50" s="43"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="14" t="s">
+      <c r="H50" s="46"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J50" s="14" t="s">
+      <c r="K50" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K50" s="14" t="s">
+      <c r="L50" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L50" s="14" t="s">
+      <c r="M50" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="N50" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>100</v>
       </c>
@@ -2404,65 +2452,67 @@
       <c r="E51" s="26">
         <v>28</v>
       </c>
-      <c r="F51" s="42" t="s">
+      <c r="F51" s="37"/>
+      <c r="G51" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="G51" s="43"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="14" t="s">
+      <c r="H51" s="46"/>
+      <c r="I51" s="47"/>
+      <c r="J51" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J51" s="14" t="s">
+      <c r="K51" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K51" s="14" t="s">
+      <c r="L51" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L51" s="14" t="s">
+      <c r="M51" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="M51" s="20" t="s">
+      <c r="N51" s="20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="37" t="s">
+    <row r="53" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="38"/>
-      <c r="C54" s="39"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="53"/>
       <c r="D54" s="13" t="s">
         <v>47</v>
       </c>
       <c r="E54" s="20"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="20"/>
+      <c r="G54" s="21"/>
       <c r="H54" s="20"/>
       <c r="I54" s="20"/>
-    </row>
-    <row r="55" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="20"/>
+    </row>
+    <row r="55" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="41"/>
+      <c r="C55" s="44"/>
       <c r="D55" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E55" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F55" s="33" t="s">
+      <c r="F55" s="41"/>
+      <c r="G55" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G55" s="34"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="35"/>
-    </row>
-    <row r="56" spans="1:13" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="41"/>
+    </row>
+    <row r="56" spans="1:14" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
         <v>91</v>
       </c>
@@ -2478,20 +2528,23 @@
       <c r="E56" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F56" s="22" t="s">
+      <c r="F56" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G56" s="22" t="s">
+      <c r="H56" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H56" s="22" t="s">
+      <c r="I56" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I56" s="22" t="s">
+      <c r="J56" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
         <v>92</v>
       </c>
@@ -2507,46 +2560,50 @@
       <c r="E57" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F57" s="22" t="s">
+      <c r="F57" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="22" t="s">
+      <c r="H57" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H57" s="22" t="s">
+      <c r="I57" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I57" s="22" t="s">
+      <c r="J57" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B58" s="40" t="s">
+      <c r="B58" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="41"/>
+      <c r="C58" s="44"/>
       <c r="D58" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="25" t="s">
+      <c r="E58" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F58" s="33" t="s">
+      <c r="F58" s="41"/>
+      <c r="G58" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="G58" s="34"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="33" t="s">
+      <c r="H58" s="40"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
-      <c r="L58" s="35"/>
-    </row>
-    <row r="59" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K58" s="40"/>
+      <c r="L58" s="40"/>
+      <c r="M58" s="41"/>
+    </row>
+    <row r="59" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>80</v>
       </c>
@@ -2560,27 +2617,30 @@
         <v>79</v>
       </c>
       <c r="E59" s="14">
+        <v>0</v>
+      </c>
+      <c r="F59" s="34">
         <v>26</v>
       </c>
-      <c r="F59" s="42" t="s">
+      <c r="G59" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="G59" s="43"/>
-      <c r="H59" s="44"/>
-      <c r="I59" s="14" t="s">
+      <c r="H59" s="46"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J59" s="14" t="s">
+      <c r="K59" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K59" s="14" t="s">
+      <c r="L59" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L59" s="14" t="s">
+      <c r="M59" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>82</v>
       </c>
@@ -2594,28 +2654,31 @@
         <v>81</v>
       </c>
       <c r="E60" s="14">
+        <v>0</v>
+      </c>
+      <c r="F60" s="34">
         <v>50</v>
       </c>
-      <c r="F60" s="58" t="s">
+      <c r="G60" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="G60" s="59"/>
-      <c r="H60" s="60"/>
-      <c r="I60" s="14" t="s">
+      <c r="H60" s="49"/>
+      <c r="I60" s="50"/>
+      <c r="J60" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J60" s="14" t="s">
+      <c r="K60" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K60" s="14" t="s">
+      <c r="L60" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L60" s="14" t="s">
+      <c r="M60" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="61" t="s">
+    <row r="63" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="38" t="s">
         <v>106</v>
       </c>
       <c r="B63" s="31" t="s">
@@ -2641,8 +2704,8 @@
       </c>
       <c r="I63" s="31"/>
     </row>
-    <row r="64" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="61" t="s">
+    <row r="64" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="38" t="s">
         <v>107</v>
       </c>
       <c r="B64" s="31" t="s">
@@ -2671,74 +2734,85 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F49:H49"/>
+  <mergeCells count="78">
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="O47:Q47"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G49:I49"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="G35:I35"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:L34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:M34"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:M29"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I58:L58"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="I46:L46"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="G55:J55"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G39:J39"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>